<commit_message>
Correcting "Mismatching sheets" comparison
</commit_message>
<xml_diff>
--- a/test_file_example_2.xlsx
+++ b/test_file_example_2.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Python\compareXLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E47AA3-467F-4375-A260-9681EB1D841E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5156039B-AAA5-461A-8DA5-F26A3499B592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="abeblio" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -406,7 +408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDE4FE7-774B-4F47-B5F4-87ED5A5FB65D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -425,4 +427,32 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17C86E3-E539-4F53-94A8-0AA530A18E8C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86E9CBF9-38A2-4D02-9AA3-32A05EAAFB95}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>